<commit_message>
Ticket 516: import product via part number, rather than display name
</commit_message>
<xml_diff>
--- a/flspsales_forecast/static/xls/Sales_forecast_template.xlsx
+++ b/flspsales_forecast/static/xls/Sales_forecast_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perryhe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\odoo-13.0\firstlight\flspsales_forecast\static\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B302D6D8-D6E2-43AB-B43B-C26D7DC819FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB060341-7792-4726-B271-1644BD57DE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="540" windowWidth="14400" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,10 +40,10 @@
     <t>Active</t>
   </si>
   <si>
-    <t>[100332-100] ASSY - A/M, ILLUMINATED SIGN C/W FRAME AND ELECTRONICS, IC</t>
-  </si>
-  <si>
     <t>Internal</t>
+  </si>
+  <si>
+    <t>100017-000</t>
   </si>
 </sst>
 </file>
@@ -439,13 +439,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="30.7265625" customWidth="1"/>
+    <col min="1" max="1" width="21.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -468,19 +473,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3">
-        <v>44349.570671296293</v>
+        <v>44450</v>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Ticket #547 - BOM Availability - bugfix
</commit_message>
<xml_diff>
--- a/flspsales_forecast/static/xls/Sales_forecast_template.xlsx
+++ b/flspsales_forecast/static/xls/Sales_forecast_template.xlsx
@@ -494,4 +494,242 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A73FFE4BB55E343861FB64325C8999A" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9896d00b689a74ff7c7bd5971296394c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="67df579b-43f8-4af9-8132-56bc3cc0d742" xmlns:ns3="96cff3de-9813-43d7-9674-16fa80042e94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="632c74f02f425a9c163423de4da529ee" ns2:_="" ns3:_="">
+    <xsd:import namespace="67df579b-43f8-4af9-8132-56bc3cc0d742"/>
+    <xsd:import namespace="96cff3de-9813-43d7-9674-16fa80042e94"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="67df579b-43f8-4af9-8132-56bc3cc0d742" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="96cff3de-9813-43d7-9674-16fa80042e94" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFB014E3-AA7D-4793-9927-A4D27C4C1E78}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5A3BFA0-BEC1-4EC6-99F5-A1BD918B509B}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC37DB91-0534-4CC5-9565-E57F2F1793AC}"/>
 </file>
</xml_diff>